<commit_message>
updated files for reference levels and newest version of demo
</commit_message>
<xml_diff>
--- a/klassegr/klassegrenser_AIP.xlsx
+++ b/klassegr/klassegrenser_AIP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nina\NatInd\2023\klassegr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\61308-01_fu_intern_hanno_sandvik\ecRxiv_vann\indicators\NO_WXXX_999\klassegr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25353B6-D606-4A5C-B5E8-E0EDD3F02D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A237728-7EC3-4FAE-A7F8-D1EC6CD2FAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3A75F986-4B69-4A9F-BCAA-E28782105059}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3A75F986-4B69-4A9F-BCAA-E28782105059}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,30 +41,6 @@
     <t>typ</t>
   </si>
   <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>SD_nedre</t>
-  </si>
-  <si>
-    <t>SD_D</t>
-  </si>
-  <si>
-    <t>D_M</t>
-  </si>
-  <si>
-    <t>M_G</t>
-  </si>
-  <si>
-    <t>G_SG</t>
-  </si>
-  <si>
-    <t>SG_øvre</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
     <t>R101</t>
   </si>
   <si>
@@ -135,6 +111,30 @@
   </si>
   <si>
     <t>R208</t>
+  </si>
+  <si>
+    <t>pess</t>
+  </si>
+  <si>
+    <t>X0</t>
+  </si>
+  <si>
+    <t>X20</t>
+  </si>
+  <si>
+    <t>X40</t>
+  </si>
+  <si>
+    <t>X60</t>
+  </si>
+  <si>
+    <t>X80</t>
+  </si>
+  <si>
+    <t>X100</t>
+  </si>
+  <si>
+    <t>opt</t>
   </si>
 </sst>
 </file>
@@ -190,9 +190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -230,7 +230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -336,7 +336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,7 +489,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,33 +499,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>5.13</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>5.13</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>5.13</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>5.13</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>5.13</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>5.13</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>5.13</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>5.13</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>5.13</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>5.13</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>5.13</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>5.13</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>5.13</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>5.13</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>5.13</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>5.13</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>5.13</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>5.13</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>5.13</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>5.13</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>5.13</v>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>5.13</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>5.13</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>5.13</v>

</xml_diff>